<commit_message>
BKP not working yet
</commit_message>
<xml_diff>
--- a/calculations/motor_calculations.xlsx
+++ b/calculations/motor_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\realslimshady\Documents\GitHub\stepper-satellite\calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDDD1829-58A1-4BED-A861-DB38B89032B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E28FDBAF-D00F-4993-94D6-9D89A46E1519}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STEPPER AND INTERUPT" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="51">
   <si>
     <t>rpm</t>
   </si>
@@ -139,9 +139,6 @@
     <t xml:space="preserve">RUNTIME BASED COUNTER CALCULATION </t>
   </si>
   <si>
-    <t>chosen runtime</t>
-  </si>
-  <si>
     <t>determined experimentally</t>
   </si>
   <si>
@@ -149,18 +146,6 @@
   </si>
   <si>
     <t>time for a full round</t>
-  </si>
-  <si>
-    <t xml:space="preserve">measured possible max runtime </t>
-  </si>
-  <si>
-    <t>possible harmonized runtime</t>
-  </si>
-  <si>
-    <t>estimated harmonization cost 4us</t>
-  </si>
-  <si>
-    <t>equal or bigger (if motor is not able to reach topspeed)</t>
   </si>
   <si>
     <t xml:space="preserve">* switch actions per step
@@ -210,6 +195,9 @@
   </si>
   <si>
     <t>min motor speed</t>
+  </si>
+  <si>
+    <t>measured average runtime</t>
   </si>
 </sst>
 </file>
@@ -432,7 +420,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -491,9 +479,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -509,6 +494,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -517,15 +511,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2044,10 +2029,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="G5:K41"/>
+  <dimension ref="G5:K39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2056,27 +2041,27 @@
     <col min="7" max="7" width="38" style="7" customWidth="1"/>
     <col min="8" max="9" width="11.42578125" style="4"/>
     <col min="10" max="10" width="21.5703125" style="10" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" style="31"/>
+    <col min="11" max="11" width="11.42578125" style="27"/>
     <col min="12" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
     <row r="5" spans="7:11" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G5" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="30"/>
+      <c r="G5" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="26"/>
     </row>
     <row r="6" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="21" t="s">
+      <c r="H6" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="22">
+      <c r="I6" s="21">
         <v>1750</v>
       </c>
       <c r="J6" s="10" t="s">
@@ -2095,7 +2080,7 @@
     </row>
     <row r="8" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G8" s="16" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H8" s="17" t="s">
         <v>2</v>
@@ -2109,7 +2094,7 @@
     </row>
     <row r="9" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G9" s="16" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>4</v>
@@ -2124,7 +2109,7 @@
     </row>
     <row r="10" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G10" s="16" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H10" s="17" t="s">
         <v>1</v>
@@ -2136,7 +2121,7 @@
     </row>
     <row r="11" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G11" s="16" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="H11" s="17" t="s">
         <v>4</v>
@@ -2145,12 +2130,12 @@
         <v>2</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G12" s="16" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H12" s="17" t="s">
         <v>3</v>
@@ -2162,7 +2147,7 @@
     </row>
     <row r="13" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G13" s="16" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H13" s="17" t="s">
         <v>4</v>
@@ -2176,7 +2161,7 @@
     </row>
     <row r="14" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G14" s="16" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H14" s="17" t="s">
         <v>3</v>
@@ -2202,256 +2187,226 @@
       <c r="K16" s="17"/>
     </row>
     <row r="18" spans="7:11" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G18" s="26" t="s">
+      <c r="G18" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="30"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="26"/>
     </row>
     <row r="19" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G19" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="H19" s="21" t="s">
+      <c r="G19" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="H19" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="I19" s="22">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="7:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="G20" s="18" t="s">
+      <c r="I19" s="12">
+        <v>9.93</v>
+      </c>
+    </row>
+    <row r="20" spans="7:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G20" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="H20" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="I20" s="25">
+        <v>100</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G21" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="I21" s="14">
+        <f>(I20/60)*I9*I11*I13</f>
+        <v>1333.3333333333335</v>
+      </c>
+    </row>
+    <row r="22" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G22" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I22" s="14">
+        <f>1/I21*10^6</f>
+        <v>749.99999999999989</v>
+      </c>
+      <c r="J22" s="11" t="s">
         <v>36</v>
-      </c>
-      <c r="H20" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="I20" s="12">
-        <f>I19+4</f>
-        <v>32</v>
-      </c>
-      <c r="J20" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="7:11" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="G21" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="H21" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="I21" s="12">
-        <f>I20</f>
-        <v>32</v>
-      </c>
-      <c r="J21" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="7:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G22" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="H22" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="I22" s="29">
-        <v>100</v>
-      </c>
-      <c r="J22" s="10" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="23" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G23" s="16" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="H23" s="17" t="s">
         <v>4</v>
       </c>
       <c r="I23" s="14">
-        <f>(I22/60)*I9*I11*I13</f>
-        <v>1333.3333333333335</v>
-      </c>
-    </row>
-    <row r="24" spans="7:11" x14ac:dyDescent="0.25">
+        <f>I22/I19</f>
+        <v>75.528700906344397</v>
+      </c>
+    </row>
+    <row r="24" spans="7:11" ht="30" x14ac:dyDescent="0.25">
       <c r="G24" s="16" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="H24" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="I24" s="14">
-        <f>1/I23*10^6</f>
-        <v>749.99999999999989</v>
-      </c>
-      <c r="J24" s="11" t="s">
-        <v>41</v>
+        <v>4</v>
+      </c>
+      <c r="I24" s="12">
+        <v>5</v>
+      </c>
+      <c r="J24" s="10" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G25" s="16" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="I25" s="14">
-        <f>I24/I21</f>
-        <v>23.437499999999996</v>
-      </c>
-    </row>
-    <row r="26" spans="7:11" ht="30" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="I25" s="15">
+        <f>I24*I19</f>
+        <v>49.65</v>
+      </c>
+    </row>
+    <row r="26" spans="7:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="G26" s="16" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="H26" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="I26" s="12">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="I26" s="15">
+        <f>I25*I13*I11</f>
+        <v>198.6</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G27" s="16" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="H27" s="17" t="s">
         <v>6</v>
       </c>
       <c r="I27" s="15">
-        <f>I26*I21</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="7:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="G28" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="H28" s="17" t="s">
+        <f>I26*I9</f>
+        <v>39720</v>
+      </c>
+      <c r="J27" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="7:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G28" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="I28" s="14">
+        <f>10^6/I27*60</f>
+        <v>1510.5740181268884</v>
+      </c>
+    </row>
+    <row r="29" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="K29" s="17"/>
+    </row>
+    <row r="33" spans="7:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="G33" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G34" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I34" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I28" s="15">
-        <f>I27*I13*I11</f>
-        <v>256</v>
-      </c>
-      <c r="J28" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G29" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="H29" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="I29" s="15">
-        <f>I28*I9</f>
-        <v>51200</v>
-      </c>
-      <c r="J29" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="7:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G30" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="H30" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="I30" s="14">
-        <f>10^6/I29*60</f>
-        <v>1171.875</v>
-      </c>
-    </row>
-    <row r="31" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="K31" s="17"/>
-    </row>
-    <row r="35" spans="7:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="G35" s="8" t="s">
-        <v>29</v>
+      <c r="I35" s="5">
+        <f>1/I34</f>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="36" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G36" s="7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I36" s="5">
-        <v>16</v>
+        <v>4</v>
+      </c>
+      <c r="I36" s="9">
+        <v>1</v>
+      </c>
+      <c r="J36" s="10" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G37" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H37" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I37" s="9">
+        <v>50</v>
+      </c>
+      <c r="J37" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="7:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G38" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H38" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I37" s="5">
-        <f>1/I36</f>
-        <v>6.25E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G38" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I38" s="9">
-        <v>1</v>
-      </c>
-      <c r="J38" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="I38" s="5">
+        <f>I35*I36*I37</f>
+        <v>3.125</v>
+      </c>
+    </row>
+    <row r="39" spans="7:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G39" s="7" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I39" s="9">
-        <v>50</v>
-      </c>
-      <c r="J39" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="40" spans="7:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G40" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H40" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I40" s="5">
-        <f>I37*I38*I39</f>
-        <v>3.125</v>
-      </c>
-    </row>
-    <row r="41" spans="7:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G41" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H41" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I41" s="5">
-        <f>1/I40*10^6/1000</f>
+      <c r="I39" s="5">
+        <f>1/I38*10^6/1000</f>
         <v>320</v>
       </c>
     </row>
@@ -2481,19 +2436,19 @@
   <sheetData>
     <row r="4" spans="5:14" ht="203.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="5:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="J7" s="28" t="s">
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="J7" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="28"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
     </row>
     <row r="9" spans="5:14" ht="60" x14ac:dyDescent="0.25">
       <c r="E9" s="1" t="s">

</xml_diff>

<commit_message>
Add atmel calculation sheet
</commit_message>
<xml_diff>
--- a/calculations/motor_calculations.xlsx
+++ b/calculations/motor_calculations.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\realslimshady\Documents\git\stepper-satellite\calculations\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D15374-0214-48F6-87FA-18C38594CB73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="STEPPER AND INTERUPT" sheetId="1" r:id="rId1"/>
@@ -228,7 +222,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -594,10 +588,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Calculation" xfId="3" builtinId="22"/>
-    <cellStyle name="Input" xfId="1" builtinId="20"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Output" xfId="2" builtinId="21"/>
+    <cellStyle name="Ausgabe" xfId="2" builtinId="21"/>
+    <cellStyle name="Berechnung" xfId="3" builtinId="22"/>
+    <cellStyle name="Eingabe" xfId="1" builtinId="20"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -613,9 +607,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -742,7 +736,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-D5DE-44E1-A6A0-82EB2F56B26B}"/>
             </c:ext>
@@ -847,7 +841,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-D5DE-44E1-A6A0-82EB2F56B26B}"/>
             </c:ext>
@@ -861,12 +855,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="874251024"/>
-        <c:axId val="524172912"/>
+        <c:axId val="56178176"/>
+        <c:axId val="56180096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="874251024"/>
+        <c:axId val="56178176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -920,26 +915,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-CH"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -974,10 +949,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CH"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="524172912"/>
+        <c:crossAx val="56180096"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -985,7 +960,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="524172912"/>
+        <c:axId val="56180096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2000"/>
@@ -1040,26 +1015,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-CH"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1091,10 +1046,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CH"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="874251024"/>
+        <c:crossAx val="56178176"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="500"/>
@@ -1144,20 +1099,20 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CH"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1181,7 +1136,7 @@
       <a:pPr>
         <a:defRPr sz="1100"/>
       </a:pPr>
-      <a:endParaRPr lang="en-CH"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1193,9 +1148,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1383,7 +1338,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-6DA2-4B5D-A793-5CC04ED6F40F}"/>
             </c:ext>
@@ -1397,11 +1352,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="148629631"/>
-        <c:axId val="150125983"/>
+        <c:axId val="56430976"/>
+        <c:axId val="56432512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="148629631"/>
+        <c:axId val="56430976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1455,15 +1410,15 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CH"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="150125983"/>
+        <c:crossAx val="56432512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="150125983"/>
+        <c:axId val="56432512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1487,7 +1442,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148629631"/>
+        <c:crossAx val="56430976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1526,20 +1481,20 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CH"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1563,7 +1518,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-CH"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2706,7 +2661,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4E223F7-F7DD-4BD3-AFEC-7F4AEB6AEE7C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D4E223F7-F7DD-4BD3-AFEC-7F4AEB6AEE7C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2742,7 +2697,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65BCECE1-55EB-41D1-B082-9EA14BF676BA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{65BCECE1-55EB-41D1-B082-9EA14BF676BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2764,9 +2719,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2804,9 +2759,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2839,26 +2794,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2891,26 +2829,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3083,14 +3004,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="G5:K39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="6" width="11.42578125" style="2"/>
     <col min="7" max="7" width="38" style="5" customWidth="1"/>
@@ -3476,14 +3397,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E4:W32"/>
   <sheetViews>
     <sheetView topLeftCell="D7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="N37" sqref="N37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="8" width="12.85546875" style="1" customWidth="1"/>
     <col min="11" max="14" width="12.85546875" style="1" customWidth="1"/>
@@ -4595,7 +4516,7 @@
       </c>
       <c r="Q24" s="30">
         <f t="shared" si="6"/>
-        <v>437.89389038085938</v>
+        <v>437.89389038085937</v>
       </c>
       <c r="R24" s="30">
         <f t="shared" si="3"/>

</xml_diff>